<commit_message>
Se corrigió el error de los separadores decimales
</commit_message>
<xml_diff>
--- a/Cuenca_conagua/uploaded_files/Escurrimiento_anual.xlsx
+++ b/Cuenca_conagua/uploaded_files/Escurrimiento_anual.xlsx
@@ -35,9 +35,6 @@
     <t>RAMIREZ</t>
   </si>
   <si>
-    <t>TEPETITALN</t>
-  </si>
-  <si>
     <t>TEPUXTEPEC</t>
   </si>
   <si>
@@ -135,6 +132,9 @@
   </si>
   <si>
     <t>Escurrimiento mensual restituido, ORIGINAL, fuente restituciones anuales CONAGUA, hm3</t>
+  </si>
+  <si>
+    <t>TEPETITLAN</t>
   </si>
 </sst>
 </file>
@@ -538,13 +538,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:19" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
@@ -558,57 +560,57 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="R3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="4">
         <v>326.44449444682868</v>
@@ -668,7 +670,7 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="6">
         <v>380.5379575468823</v>
@@ -728,7 +730,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="6">
         <v>388.04114595183279</v>
@@ -788,7 +790,7 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="6">
         <v>352.19505195183268</v>
@@ -848,7 +850,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="6">
         <v>483.17403095183272</v>
@@ -908,7 +910,7 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="7">
         <v>399.73373113269469</v>
@@ -968,7 +970,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="6">
         <v>319.51250755666666</v>
@@ -1028,7 +1030,7 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="6">
         <v>304.90797370000001</v>
@@ -1088,7 +1090,7 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="6">
         <v>401.29621151912539</v>
@@ -1148,7 +1150,7 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="6">
         <v>318.00440075331716</v>
@@ -1208,7 +1210,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" s="6">
         <v>336.69501618764713</v>
@@ -1268,7 +1270,7 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="6">
         <v>714.0317051162549</v>
@@ -1328,7 +1330,7 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" s="6">
         <v>334.12275533928403</v>
@@ -1388,7 +1390,7 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" s="6">
         <v>294.91263084177427</v>
@@ -1448,7 +1450,7 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18" s="6">
         <v>349.95107290695245</v>
@@ -1508,7 +1510,7 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B19" s="6">
         <v>363.97155195887376</v>
@@ -1568,7 +1570,7 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B20" s="8">
         <v>400.72421245192356</v>
@@ -1628,5 +1630,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>